<commit_message>
Final stage of my project, I missed the serialization. Nevertheless, I added the complete documentation, a javadoc, the save game function, and corrected some issues.
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y Trazabilidad.xlsx
+++ b/docs/Requerimientos y Trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\catch-Pac-Man\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E145CD-1D85-4BC2-A277-D0CFB772F243}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469CB9E3-B377-40E8-9211-F15CDA4866D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{31C48E74-0393-49E3-B191-A28F62AD17B8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>R1</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>saveGame(ActionEvent)</t>
+  </si>
+  <si>
+    <t>getSavedGame(ActionEvent)</t>
+  </si>
+  <si>
+    <t>showScores(ActionEvent)</t>
   </si>
 </sst>
 </file>
@@ -220,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -280,11 +286,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -311,6 +328,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -629,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2BE07B-8EDE-4BB5-9907-C48003AE6E24}">
   <dimension ref="G6:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,15 +898,11 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="7:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="G24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>34</v>
+    <row r="24" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -892,14 +911,14 @@
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="2" t="s">
+      <c r="G25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>44</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -908,11 +927,11 @@
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="M26" s="1"/>
@@ -921,10 +940,14 @@
     </row>
     <row r="27" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="M27" s="1"/>
@@ -933,7 +956,7 @@
     </row>
     <row r="28" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G28" s="2" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -945,29 +968,50 @@
     </row>
     <row r="29" spans="7:15" x14ac:dyDescent="0.3">
       <c r="G29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G31" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
     <row r="32" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G32" s="11"/>
+      <c r="H32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -983,11 +1027,14 @@
       <c r="O34" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="G31:G32"/>
     <mergeCell ref="G6:K6"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="H19:H23"/>
-    <mergeCell ref="G19:G23"/>
+    <mergeCell ref="G19:G24"/>
+    <mergeCell ref="H19:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Now the PacMan can be stopped
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y Trazabilidad.xlsx
+++ b/docs/Requerimientos y Trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\catch-Pac-Man\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469CB9E3-B377-40E8-9211-F15CDA4866D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6488E7-B335-4DFB-8034-484FD640DF38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{31C48E74-0393-49E3-B191-A28F62AD17B8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="53">
   <si>
     <t>R1</t>
   </si>
@@ -195,7 +195,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,16 +217,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -235,106 +291,67 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -342,6 +359,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -650,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2BE07B-8EDE-4BB5-9907-C48003AE6E24}">
-  <dimension ref="G6:O34"/>
+  <dimension ref="G5:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,216 +690,217 @@
     <col min="15" max="15" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G6" s="5" t="s">
+    <row r="5" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="7:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G7" s="2" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="7:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="7:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="G8" s="2" t="s">
+    <row r="8" spans="7:11" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="7:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="G9" s="2" t="s">
+    <row r="9" spans="7:11" ht="73.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="7:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="G10" s="2" t="s">
+    <row r="10" spans="7:11" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="7:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="G11" s="2" t="s">
+    <row r="11" spans="7:11" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="7:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="G12" s="2" t="s">
+    <row r="12" spans="7:11" ht="73.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2" t="s">
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="7:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="G13" s="2" t="s">
+    <row r="13" spans="7:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="7:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="G14" s="2" t="s">
+    <row r="14" spans="7:11" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="7:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G17" s="6" t="s">
+    <row r="17" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G18" s="4" t="s">
+    <row r="18" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G19" s="9" t="s">
+    <row r="19" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="5" t="s">
         <v>34</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="2" t="s">
+    <row r="20" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5" t="s">
         <v>35</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="2" t="s">
+    <row r="21" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="5" t="s">
         <v>47</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="2" t="s">
+    <row r="22" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="5" t="s">
         <v>48</v>
       </c>
       <c r="J22" s="1"/>
@@ -886,10 +909,10 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="2" t="s">
+    <row r="23" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J23" s="1"/>
@@ -898,10 +921,10 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10" t="s">
+    <row r="24" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="5" t="s">
         <v>51</v>
       </c>
       <c r="J24" s="1"/>
@@ -910,14 +933,14 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G25" s="11" t="s">
+    <row r="25" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="7" t="s">
         <v>34</v>
       </c>
       <c r="J25" s="1"/>
@@ -926,10 +949,10 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="2" t="s">
+    <row r="26" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7" t="s">
         <v>50</v>
       </c>
       <c r="J26" s="1"/>
@@ -938,14 +961,14 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G27" s="2" t="s">
+    <row r="27" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G27" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="8" t="s">
         <v>50</v>
       </c>
       <c r="J27" s="1"/>
@@ -954,69 +977,69 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G28" s="2" t="s">
+    <row r="28" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G28" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G29" s="2" t="s">
+    <row r="29" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G29" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="7:15" x14ac:dyDescent="0.3">
-      <c r="G30" s="2" t="s">
+    <row r="30" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G30" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="10" t="s">
         <v>52</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="7:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G31" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="12" t="s">
         <v>46</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="7:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G32" s="11"/>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="12" t="s">
         <v>35</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="13:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>

</xml_diff>

<commit_message>
The game can now be serialized and I added a requirement. This is the latest coded version of the program
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y Trazabilidad.xlsx
+++ b/docs/Requerimientos y Trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\catch-Pac-Man\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6488E7-B335-4DFB-8034-484FD640DF38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBC29F6-1C57-4991-AB64-114B3C073BBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{31C48E74-0393-49E3-B191-A28F62AD17B8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>R1</t>
   </si>
@@ -110,12 +110,6 @@
     <t>Serealización</t>
   </si>
   <si>
-    <t>Permite que la lectura y escritura de los puntajes se lleve a cabo por medio de serealización. De esta forma, impidiendo la manipulación de los mismos por parte de los usuarios.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los puntajes son serializados </t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
@@ -189,6 +183,30 @@
   </si>
   <si>
     <t>showScores(ActionEvent)</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Parar PacMan</t>
+  </si>
+  <si>
+    <t>Al hacer click sobre un PacMan, este debe detenerse</t>
+  </si>
+  <si>
+    <t>Ubicacion en X y en Y del click</t>
+  </si>
+  <si>
+    <t>El PacMan está detenido</t>
+  </si>
+  <si>
+    <t>stopPacMan(ActionEvent)</t>
+  </si>
+  <si>
+    <t>Permite la serialización del estado actual del juego cuando el usuario presiona "Guardar Juego"</t>
+  </si>
+  <si>
+    <t>El juego serializado y guardado</t>
   </si>
 </sst>
 </file>
@@ -226,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,8 +299,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -305,53 +335,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2BE07B-8EDE-4BB5-9907-C48003AE6E24}">
-  <dimension ref="G5:O34"/>
+  <dimension ref="G2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,147 +772,165 @@
     <col min="15" max="15" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="7:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G6" s="14" t="s">
+    <row r="2" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="7:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="7:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="7:11" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="7:11" ht="73.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="7:11" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="7:11" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="7:11" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="7:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="7:11" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" spans="7:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="7:11" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="7:11" ht="73.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="7:11" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="7:11" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="7:11" ht="73.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="7:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="7:11" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G14" s="9" t="s">
+      <c r="H11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="J11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="K11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="7:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="7:11" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -845,63 +945,63 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="G17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>33</v>
+      <c r="H18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>34</v>
+      <c r="H19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5" t="s">
-        <v>35</v>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5" t="s">
-        <v>47</v>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="5" t="s">
-        <v>48</v>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -910,10 +1010,10 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="5" t="s">
-        <v>49</v>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -922,10 +1022,10 @@
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="5" t="s">
-        <v>51</v>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -934,14 +1034,14 @@
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>34</v>
+      <c r="H25" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -950,10 +1050,10 @@
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="7" t="s">
-        <v>50</v>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -962,14 +1062,14 @@
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H27" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>50</v>
+      <c r="H27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -978,11 +1078,11 @@
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="M28" s="1"/>
@@ -990,71 +1090,84 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
+      <c r="G29" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G30" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>52</v>
+      <c r="G30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G31" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>46</v>
+      <c r="G31" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
     <row r="32" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="11"/>
-      <c r="H32" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>35</v>
+      <c r="G32" s="15"/>
+      <c r="H32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="13:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>56</v>
+      </c>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="13:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G3:K3"/>
     <mergeCell ref="G25:G26"/>
     <mergeCell ref="H25:H26"/>
     <mergeCell ref="G31:G32"/>
-    <mergeCell ref="G6:K6"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="G19:G24"/>
     <mergeCell ref="H19:H24"/>

</xml_diff>